<commit_message>
Lots more graphics pulled out, palettes made readable
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9765" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="9765" windowHeight="9195" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Splash sound" sheetId="2" r:id="rId2"/>
     <sheet name="Splash tile data" sheetId="3" r:id="rId3"/>
+    <sheet name="Palette" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="148">
   <si>
     <t>0f0e0f0e0d0e0e0f</t>
   </si>
@@ -433,6 +434,39 @@
   </si>
   <si>
     <t>1A</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>JASC-PAL</t>
+  </si>
+  <si>
+    <t>00 17 0D 00 39 15 2A 3F 0B 00 00 00 00 00 00 00</t>
+  </si>
+  <si>
+    <t>0100</t>
   </si>
 </sst>
 </file>
@@ -937,11 +971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="312452632"/>
-        <c:axId val="312454200"/>
+        <c:axId val="474209832"/>
+        <c:axId val="474210224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="312452632"/>
+        <c:axId val="474209832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +1017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312454200"/>
+        <c:crossAx val="474210224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -991,7 +1025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312454200"/>
+        <c:axId val="474210224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1043,7 +1077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312452632"/>
+        <c:crossAx val="474209832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1107,7 +1141,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1466,11 +1499,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="312452240"/>
-        <c:axId val="312453024"/>
+        <c:axId val="474211400"/>
+        <c:axId val="474212184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="312452240"/>
+        <c:axId val="474211400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312453024"/>
+        <c:crossAx val="474212184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1520,7 +1553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="312453024"/>
+        <c:axId val="474212184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,7 +1604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="312452240"/>
+        <c:crossAx val="474211400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5745,8 +5778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22255,4 +22288,2402 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="22" width="4.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" t="s">
+        <v>143</v>
+      </c>
+      <c r="O2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>138</v>
+      </c>
+      <c r="R2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S2" t="s">
+        <v>140</v>
+      </c>
+      <c r="T2" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" t="s">
+        <v>139</v>
+      </c>
+      <c r="V2" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <f>(ROW()-ROW($B$3))*6+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>HEX2DEC(MID($B$1,$B3,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>HEX2DEC(MID($B$1,$B3+1,1))</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>HEX2DEC(MID($B$1,$B3+3,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>E3*255/15</f>
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <f>D3*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>C3*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <f>"  GGCOLOUR $"&amp;DEC2HEX(F3*65536+G3*256+H3,6)</f>
+        <v xml:space="preserve">  GGCOLOUR $110000</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="0">(ROW()-ROW($B$3))*3+1</f>
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P12" si="1">HEX2DEC(MID($B$1,O3,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q12" si="2">_xlfn.BITAND(P3,3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R12" si="3">_xlfn.BITAND(_xlfn.BITRSHIFT(P3,2),3)</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S12" si="4">_xlfn.BITAND(_xlfn.BITRSHIFT(P3,4),3)</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T12" si="5">Q3*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U12" si="6">R3*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V12" si="7">S3*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="W3" t="str">
+        <f>"  SMSCOLOUR $"&amp;DEC2HEX(T3*65536+U3*256+V3,6)</f>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <f>(ROW()-ROW($B$3))*6+1</f>
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <f>HEX2DEC(MID($B$1,$B4,1))</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>HEX2DEC(MID($B$1,$B4+1,1))</f>
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <f>HEX2DEC(MID($B$1,$B4+3,1))</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>E4*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>D4*255/15</f>
+        <v>221</v>
+      </c>
+      <c r="H4">
+        <f>C4*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <f>"  GGCOLOUR $"&amp;DEC2HEX(F4*65536+G4*256+H4,6)</f>
+        <v xml:space="preserve">  GGCOLOUR $00DD00</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" ref="W4:W12" si="8">"  SMSCOLOUR $"&amp;DEC2HEX(T4*65536+U4*256+V4,6)</f>
+        <v xml:space="preserve">  SMSCOLOUR $FF5555</v>
+      </c>
+      <c r="AA4" t="str">
+        <f>T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <f t="shared" ref="B5:B34" si="9">(ROW()-ROW($B$3))*6+1</f>
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C34" si="10">HEX2DEC(MID($B$1,$B5,1))</f>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D34" si="11">HEX2DEC(MID($B$1,$B5+1,1))</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E34" si="12">HEX2DEC(MID($B$1,$B5+3,1))</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F34" si="13">E5*255/15</f>
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G22" si="14">D5*255/15</f>
+        <v>153</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H22" si="15">C5*255/15</f>
+        <v>51</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:I22" si="16">"  GGCOLOUR $"&amp;DEC2HEX(F5*65536+G5*256+H5,6)</f>
+        <v xml:space="preserve">  GGCOLOUR $119933</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W5" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $55FF00</v>
+      </c>
+      <c r="AA5" t="str">
+        <f>T4&amp;" "&amp;U4&amp;" "&amp;V4</f>
+        <v>255 85 85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="13"/>
+        <v>51</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="14"/>
+        <v>170</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="15"/>
+        <v>34</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $33AA22</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA6" t="str">
+        <f>T5&amp;" "&amp;U5&amp;" "&amp;V5</f>
+        <v>85 255 0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="14"/>
+        <v>187</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $00BB00</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $55AAFF</v>
+      </c>
+      <c r="AA7" t="str">
+        <f>T6&amp;" "&amp;U6&amp;" "&amp;V6</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <f t="shared" si="9"/>
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="5"/>
+        <v>85</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="W8" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $555555</v>
+      </c>
+      <c r="AA8" t="str">
+        <f>T7&amp;" "&amp;U7&amp;" "&amp;V7</f>
+        <v>85 170 255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <f t="shared" si="9"/>
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="7"/>
+        <v>170</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $AAAAAA</v>
+      </c>
+      <c r="AA9" t="str">
+        <f>T8&amp;" "&amp;U8&amp;" "&amp;V8</f>
+        <v>85 85 85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <f t="shared" si="9"/>
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $FFFFFF</v>
+      </c>
+      <c r="AA10" t="str">
+        <f>T9&amp;" "&amp;U9&amp;" "&amp;V9</f>
+        <v>170 170 170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $FFAA00</v>
+      </c>
+      <c r="AA11" t="str">
+        <f>T10&amp;" "&amp;U10&amp;" "&amp;V10</f>
+        <v>255 255 255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <f t="shared" si="9"/>
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA12" t="str">
+        <f>T11&amp;" "&amp;U11&amp;" "&amp;V11</f>
+        <v>255 170 0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <f t="shared" si="9"/>
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ref="O13:O34" si="17">(ROW()-ROW($B$3))*3+1</f>
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P34" si="18">HEX2DEC(MID($B$1,O13,2))</f>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13:Q34" si="19">_xlfn.BITAND(P13,3)</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ref="R13:R34" si="20">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13:S34" si="21">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ref="T13:T34" si="22">Q13*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f t="shared" ref="U13:U34" si="23">R13*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f t="shared" ref="V13:V34" si="24">S13*255/3</f>
+        <v>0</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" ref="W13:W34" si="25">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA13" t="str">
+        <f>T12&amp;" "&amp;U12&amp;" "&amp;V12</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <f t="shared" si="9"/>
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="17"/>
+        <v>34</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA14" t="str">
+        <f>T13&amp;" "&amp;U13&amp;" "&amp;V13</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <f t="shared" si="9"/>
+        <v>73</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="17"/>
+        <v>37</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA15" t="str">
+        <f>T14&amp;" "&amp;U14&amp;" "&amp;V14</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <f t="shared" si="9"/>
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA16" t="str">
+        <f>T15&amp;" "&amp;U15&amp;" "&amp;V15</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <f t="shared" si="9"/>
+        <v>85</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="17"/>
+        <v>43</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA17" t="str">
+        <f>T16&amp;" "&amp;U16&amp;" "&amp;V16</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <f t="shared" si="9"/>
+        <v>91</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="17"/>
+        <v>46</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA18" t="str">
+        <f>T17&amp;" "&amp;U17&amp;" "&amp;V17</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <f t="shared" si="9"/>
+        <v>97</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="17"/>
+        <v>49</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA19" t="str">
+        <f>T18&amp;" "&amp;U18&amp;" "&amp;V18</f>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <f t="shared" si="9"/>
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="17"/>
+        <v>52</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <f t="shared" si="9"/>
+        <v>109</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="17"/>
+        <v>55</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <f t="shared" si="9"/>
+        <v>115</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="17"/>
+        <v>58</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W22" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <f t="shared" si="9"/>
+        <v>121</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G34" si="26">D23*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H34" si="27">C23*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" ref="I23:I34" si="28">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="17"/>
+        <v>61</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W23" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <f t="shared" si="9"/>
+        <v>127</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="17"/>
+        <v>64</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W24" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <f t="shared" si="9"/>
+        <v>133</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="17"/>
+        <v>67</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W25" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <f t="shared" si="9"/>
+        <v>139</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="17"/>
+        <v>70</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W26" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <f t="shared" si="9"/>
+        <v>145</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="17"/>
+        <v>73</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W27" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <f t="shared" si="9"/>
+        <v>151</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="17"/>
+        <v>76</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W28" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <f t="shared" si="9"/>
+        <v>157</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="17"/>
+        <v>79</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W29" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <f t="shared" si="9"/>
+        <v>163</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="17"/>
+        <v>82</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W30" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <f t="shared" si="9"/>
+        <v>169</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="17"/>
+        <v>85</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W31" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <f t="shared" si="9"/>
+        <v>175</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="17"/>
+        <v>88</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W32" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <f t="shared" si="9"/>
+        <v>181</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="17"/>
+        <v>91</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W33" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <f t="shared" si="9"/>
+        <v>187</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="28"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="17"/>
+        <v>94</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="W34" t="str">
+        <f t="shared" si="25"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Powerboats track data extracted
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -971,11 +971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="474209832"/>
-        <c:axId val="474210224"/>
+        <c:axId val="512945704"/>
+        <c:axId val="512941784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474209832"/>
+        <c:axId val="512945704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474210224"/>
+        <c:crossAx val="512941784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474210224"/>
+        <c:axId val="512941784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1077,7 +1077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474209832"/>
+        <c:crossAx val="512945704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1499,11 +1499,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="474211400"/>
-        <c:axId val="474212184"/>
+        <c:axId val="512948056"/>
+        <c:axId val="512942568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474211400"/>
+        <c:axId val="512948056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +1545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474212184"/>
+        <c:crossAx val="512942568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +1553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474212184"/>
+        <c:axId val="512942568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474211400"/>
+        <c:crossAx val="512948056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22519,13 +22519,13 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA4" t="str">
-        <f>T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
+        <f t="shared" ref="AA4:AA19" si="12">T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5">
-        <f t="shared" ref="B5:B34" si="12">(ROW()-ROW($B$3))*6+1</f>
+        <f t="shared" ref="B5:B34" si="13">(ROW()-ROW($B$3))*6+1</f>
         <v>13</v>
       </c>
       <c r="C5">
@@ -22541,19 +22541,19 @@
         <v>8</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F34" si="13">E5*255/15</f>
+        <f t="shared" ref="F5:F34" si="14">E5*255/15</f>
         <v>136</v>
       </c>
       <c r="G5">
-        <f t="shared" ref="G5:G22" si="14">D5*255/15</f>
+        <f t="shared" ref="G5:G22" si="15">D5*255/15</f>
         <v>68</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H22" si="15">C5*255/15</f>
+        <f t="shared" ref="H5:H22" si="16">C5*255/15</f>
         <v>0</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I22" si="16">"  GGCOLOUR $"&amp;DEC2HEX(F5*65536+G5*256+H5,6)</f>
+        <f t="shared" ref="I5:I22" si="17">"  GGCOLOUR $"&amp;DEC2HEX(F5*65536+G5*256+H5,6)</f>
         <v xml:space="preserve">  GGCOLOUR $884400</v>
       </c>
       <c r="O5">
@@ -22593,13 +22593,13 @@
         <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
       <c r="AA5" t="str">
-        <f>T4&amp;" "&amp;U4&amp;" "&amp;V4</f>
+        <f t="shared" si="12"/>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="C6">
@@ -22615,19 +22615,19 @@
         <v>14</v>
       </c>
       <c r="F6">
-        <f t="shared" si="13"/>
-        <v>238</v>
-      </c>
-      <c r="G6">
         <f t="shared" si="14"/>
         <v>238</v>
       </c>
-      <c r="H6">
+      <c r="G6">
         <f t="shared" si="15"/>
         <v>238</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="16"/>
+        <v>238</v>
+      </c>
       <c r="I6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
       </c>
       <c r="O6">
@@ -22667,13 +22667,13 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA6" t="str">
-        <f>T5&amp;" "&amp;U5&amp;" "&amp;V5</f>
+        <f t="shared" si="12"/>
         <v>0 85 0</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="C7">
@@ -22689,19 +22689,19 @@
         <v>8</v>
       </c>
       <c r="F7">
-        <f t="shared" si="13"/>
-        <v>136</v>
-      </c>
-      <c r="G7">
         <f t="shared" si="14"/>
         <v>136</v>
       </c>
-      <c r="H7">
+      <c r="G7">
         <f t="shared" si="15"/>
         <v>136</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="16"/>
+        <v>136</v>
+      </c>
       <c r="I7" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $888888</v>
       </c>
       <c r="O7">
@@ -22741,13 +22741,13 @@
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA7" t="str">
-        <f>T6&amp;" "&amp;U6&amp;" "&amp;V6</f>
+        <f t="shared" si="12"/>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>31</v>
       </c>
       <c r="C8">
@@ -22763,19 +22763,19 @@
         <v>4</v>
       </c>
       <c r="F8">
-        <f t="shared" si="13"/>
-        <v>68</v>
-      </c>
-      <c r="G8">
         <f t="shared" si="14"/>
         <v>68</v>
       </c>
-      <c r="H8">
+      <c r="G8">
         <f t="shared" si="15"/>
         <v>68</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="16"/>
+        <v>68</v>
+      </c>
       <c r="I8" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $444444</v>
       </c>
       <c r="O8">
@@ -22815,13 +22815,13 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA8" t="str">
-        <f>T7&amp;" "&amp;U7&amp;" "&amp;V7</f>
+        <f t="shared" si="12"/>
         <v>0 170 0</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="C9">
@@ -22837,19 +22837,19 @@
         <v>8</v>
       </c>
       <c r="F9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>136</v>
       </c>
       <c r="G9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $880000</v>
       </c>
       <c r="O9">
@@ -22889,13 +22889,13 @@
         <v xml:space="preserve">  SMSCOLOUR $AAFFAA</v>
       </c>
       <c r="AA9" t="str">
-        <f>T8&amp;" "&amp;U8&amp;" "&amp;V8</f>
+        <f t="shared" si="12"/>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43</v>
       </c>
       <c r="C10">
@@ -22911,19 +22911,19 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>68</v>
       </c>
       <c r="H10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>136</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $004488</v>
       </c>
       <c r="O10">
@@ -22963,13 +22963,13 @@
         <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA10" t="str">
-        <f>T9&amp;" "&amp;U9&amp;" "&amp;V9</f>
+        <f t="shared" si="12"/>
         <v>170 255 170</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>49</v>
       </c>
       <c r="C11">
@@ -22985,19 +22985,19 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O11">
@@ -23037,13 +23037,13 @@
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA11" t="str">
-        <f>T10&amp;" "&amp;U10&amp;" "&amp;V10</f>
+        <f t="shared" si="12"/>
         <v>170 255 0</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>55</v>
       </c>
       <c r="C12">
@@ -23059,19 +23059,19 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O12">
@@ -23111,13 +23111,13 @@
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA12" t="str">
-        <f>T11&amp;" "&amp;U11&amp;" "&amp;V11</f>
+        <f t="shared" si="12"/>
         <v>0 170 0</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
       <c r="C13">
@@ -23133,65 +23133,65 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O34" si="17">(ROW()-ROW($B$3))*3+1</f>
+        <f t="shared" ref="O13:O34" si="18">(ROW()-ROW($B$3))*3+1</f>
         <v>31</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P34" si="18">HEX2DEC(MID($B$1,O13,2))</f>
+        <f t="shared" ref="P13:P34" si="19">HEX2DEC(MID($B$1,O13,2))</f>
         <v>68</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13:Q34" si="19">_xlfn.BITAND(P13,3)</f>
+        <f t="shared" ref="Q13:Q34" si="20">_xlfn.BITAND(P13,3)</f>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13:R34" si="20">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
+        <f t="shared" ref="R13:R34" si="21">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
         <v>1</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:S34" si="21">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
+        <f t="shared" ref="S13:S34" si="22">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13:T34" si="22">Q13*255/3</f>
+        <f t="shared" ref="T13:T34" si="23">Q13*255/3</f>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" ref="U13:U34" si="23">R13*255/3</f>
+        <f t="shared" ref="U13:U34" si="24">R13*255/3</f>
         <v>85</v>
       </c>
       <c r="V13">
-        <f t="shared" ref="V13:V34" si="24">S13*255/3</f>
+        <f t="shared" ref="V13:V34" si="25">S13*255/3</f>
         <v>0</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" ref="W13:W34" si="25">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
+        <f t="shared" ref="W13:W34" si="26">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
         <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
       <c r="AA13" t="str">
-        <f>T12&amp;" "&amp;U12&amp;" "&amp;V12</f>
+        <f t="shared" si="12"/>
         <v>0 170 0</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>67</v>
       </c>
       <c r="C14">
@@ -23207,65 +23207,65 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>34</v>
       </c>
       <c r="P14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>85</v>
       </c>
       <c r="V14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W14" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
       <c r="AA14" t="str">
-        <f>T13&amp;" "&amp;U13&amp;" "&amp;V13</f>
+        <f t="shared" si="12"/>
         <v>0 85 0</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>73</v>
       </c>
       <c r="C15">
@@ -23281,65 +23281,65 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>37</v>
       </c>
       <c r="P15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="S15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>170</v>
       </c>
       <c r="V15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W15" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA15" t="str">
-        <f>T14&amp;" "&amp;U14&amp;" "&amp;V14</f>
+        <f t="shared" si="12"/>
         <v>0 85 0</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>79</v>
       </c>
       <c r="C16">
@@ -23355,65 +23355,65 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>40</v>
       </c>
       <c r="P16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA16" t="str">
-        <f>T15&amp;" "&amp;U15&amp;" "&amp;V15</f>
+        <f t="shared" si="12"/>
         <v>0 170 0</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>85</v>
       </c>
       <c r="C17">
@@ -23429,65 +23429,65 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>43</v>
       </c>
       <c r="P17">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>64</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R17">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V17">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W17" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA17" t="str">
-        <f>T16&amp;" "&amp;U16&amp;" "&amp;V16</f>
+        <f t="shared" si="12"/>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="C18">
@@ -23503,65 +23503,65 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>46</v>
       </c>
       <c r="P18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R18">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="S18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>170</v>
       </c>
       <c r="V18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W18" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA18" t="str">
-        <f>T17&amp;" "&amp;U17&amp;" "&amp;V17</f>
+        <f t="shared" si="12"/>
         <v>0 0 0</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>97</v>
       </c>
       <c r="C19">
@@ -23577,65 +23577,65 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O19">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>49</v>
       </c>
       <c r="P19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W19" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA19" t="str">
-        <f>T18&amp;" "&amp;U18&amp;" "&amp;V18</f>
+        <f t="shared" si="12"/>
         <v>0 170 0</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>103</v>
       </c>
       <c r="C20">
@@ -23651,61 +23651,61 @@
         <v>14</v>
       </c>
       <c r="F20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>238</v>
       </c>
       <c r="G20">
-        <f t="shared" si="14"/>
-        <v>68</v>
-      </c>
-      <c r="H20">
         <f t="shared" si="15"/>
         <v>68</v>
       </c>
+      <c r="H20">
+        <f t="shared" si="16"/>
+        <v>68</v>
+      </c>
       <c r="I20" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $EE4444</v>
       </c>
       <c r="O20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>52</v>
       </c>
       <c r="P20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T20">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W20" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>109</v>
       </c>
       <c r="C21">
@@ -23721,61 +23721,61 @@
         <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>68</v>
       </c>
       <c r="G21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>238</v>
       </c>
       <c r="H21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $44EE00</v>
       </c>
       <c r="O21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>55</v>
       </c>
       <c r="P21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U21">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W21" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>115</v>
       </c>
       <c r="C22">
@@ -23791,61 +23791,61 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>58</v>
       </c>
       <c r="P22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>121</v>
       </c>
       <c r="C23">
@@ -23861,61 +23861,61 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>68</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G34" si="26">D23*255/15</f>
+        <f t="shared" ref="G23:G34" si="27">D23*255/15</f>
         <v>136</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H34" si="27">C23*255/15</f>
+        <f t="shared" ref="H23:H34" si="28">C23*255/15</f>
         <v>238</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23:I34" si="28">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
+        <f t="shared" ref="I23:I34" si="29">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
         <v xml:space="preserve">  GGCOLOUR $4488EE</v>
       </c>
       <c r="O23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>61</v>
       </c>
       <c r="P23">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>127</v>
       </c>
       <c r="C24">
@@ -23931,61 +23931,61 @@
         <v>4</v>
       </c>
       <c r="F24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>68</v>
       </c>
       <c r="G24">
-        <f t="shared" si="26"/>
-        <v>68</v>
-      </c>
-      <c r="H24">
         <f t="shared" si="27"/>
         <v>68</v>
       </c>
+      <c r="H24">
+        <f t="shared" si="28"/>
+        <v>68</v>
+      </c>
       <c r="I24" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">  GGCOLOUR $444444</v>
       </c>
       <c r="O24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>64</v>
       </c>
       <c r="P24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W24" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>133</v>
       </c>
       <c r="C25">
@@ -24001,61 +24001,61 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>136</v>
       </c>
       <c r="G25">
-        <f t="shared" si="26"/>
-        <v>136</v>
-      </c>
-      <c r="H25">
         <f t="shared" si="27"/>
         <v>136</v>
       </c>
+      <c r="H25">
+        <f t="shared" si="28"/>
+        <v>136</v>
+      </c>
       <c r="I25" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">  GGCOLOUR $888888</v>
       </c>
       <c r="O25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>67</v>
       </c>
       <c r="P25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>139</v>
       </c>
       <c r="C26">
@@ -24071,61 +24071,61 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>238</v>
       </c>
       <c r="G26">
-        <f t="shared" si="26"/>
-        <v>238</v>
-      </c>
-      <c r="H26">
         <f t="shared" si="27"/>
         <v>238</v>
       </c>
+      <c r="H26">
+        <f t="shared" si="28"/>
+        <v>238</v>
+      </c>
       <c r="I26" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
       </c>
       <c r="O26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>70</v>
       </c>
       <c r="P26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W26" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>145</v>
       </c>
       <c r="C27">
@@ -24141,61 +24141,61 @@
         <v>14</v>
       </c>
       <c r="F27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>238</v>
       </c>
       <c r="G27">
+        <f t="shared" si="27"/>
+        <v>136</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="18"/>
+        <v>73</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W27" t="str">
         <f t="shared" si="26"/>
-        <v>136</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="17"/>
-        <v>73</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W27" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>151</v>
       </c>
       <c r="C28">
@@ -24211,61 +24211,61 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G28">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="18"/>
+        <v>76</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W28" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="17"/>
-        <v>76</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W28" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B29">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>157</v>
       </c>
       <c r="C29">
@@ -24281,61 +24281,61 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G29">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="18"/>
+        <v>79</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W29" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="17"/>
-        <v>79</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W29" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>163</v>
       </c>
       <c r="C30">
@@ -24351,61 +24351,61 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G30">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="18"/>
+        <v>82</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W30" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="17"/>
-        <v>82</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W30" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>169</v>
       </c>
       <c r="C31">
@@ -24421,61 +24421,61 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G31">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="18"/>
+        <v>85</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W31" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="17"/>
-        <v>85</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W31" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="32" spans="2:27" x14ac:dyDescent="0.45">
       <c r="B32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>175</v>
       </c>
       <c r="C32">
@@ -24491,61 +24491,61 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G32">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="18"/>
+        <v>88</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W32" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="17"/>
-        <v>88</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W32" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>181</v>
       </c>
       <c r="C33">
@@ -24561,61 +24561,61 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G33">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="18"/>
+        <v>91</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W33" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="17"/>
-        <v>91</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W33" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>187</v>
       </c>
       <c r="C34">
@@ -24631,55 +24631,55 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G34">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="18"/>
+        <v>94</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="W34" t="str">
         <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="I34" t="str">
-        <f t="shared" si="28"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="17"/>
-        <v>94</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="V34">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="W34" t="str">
-        <f t="shared" si="25"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More graphics, extracting tilemaps
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="148">
   <si>
     <t>0f0e0f0e0d0e0e0f</t>
   </si>
@@ -466,7 +466,7 @@
     <t>0100</t>
   </si>
   <si>
-    <t>00 00 44 00 48 00 EE 0E 88 08 44 04 08 00 40 08 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 4E 04 E4 00 00 00 84 0E 44 04 88 08 EE 0E 8E 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00</t>
+    <t>04 08 EE 0E 80 00 08 00 4E 04 8E 00 44 0E 00 00 22 02 44 04 88 08 40 00 C0 00 E0 00 AE 0A 00 00 04 08 EE 0E 80 00 08 00 4E 04 8E 00 88 0E 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00</t>
   </si>
 </sst>
 </file>
@@ -22292,29 +22292,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="22" width="4.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>147</v>
       </c>
-      <c r="AA1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -22372,18 +22367,21 @@
       <c r="W2" t="s">
         <v>142</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="AA2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B3">
         <f>(ROW()-ROW($B$3))*6+1</f>
         <v>1</v>
       </c>
       <c r="C3">
         <f>HEX2DEC(MID($B$1,$B3+4,1))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <f>HEX2DEC(MID($B$1,$B3+0,1))</f>
@@ -22391,11 +22389,11 @@
       </c>
       <c r="E3">
         <f>HEX2DEC(MID($B$1,$B3+1,1))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <f>E3*255/15</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G3">
         <f>D3*255/15</f>
@@ -22403,11 +22401,11 @@
       </c>
       <c r="H3">
         <f>C3*255/15</f>
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="I3" t="str">
         <f>"  GGCOLOUR $"&amp;DEC2HEX(F3*65536+G3*256+H3,6)</f>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $440088</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O12" si="0">(ROW()-ROW($B$3))*3+1</f>
@@ -22415,7 +22413,7 @@
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P12" si="1">HEX2DEC(MID($B$1,O3,2))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q12" si="2">_xlfn.BITAND(P3,3)</f>
@@ -22423,7 +22421,7 @@
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R12" si="3">_xlfn.BITAND(_xlfn.BITRSHIFT(P3,2),3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S12" si="4">_xlfn.BITAND(_xlfn.BITRSHIFT(P3,4),3)</f>
@@ -22435,7 +22433,7 @@
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U12" si="6">R3*255/3</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V12" si="7">S3*255/3</f>
@@ -22443,44 +22441,47 @@
       </c>
       <c r="W3" t="str">
         <f>"  SMSCOLOUR $"&amp;DEC2HEX(T3*65536+U3*256+V3,6)</f>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-      <c r="AA3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B4">
         <f>(ROW()-ROW($B$3))*6+1</f>
         <v>7</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C34" si="8">HEX2DEC(MID($B$1,$B4+4,1))</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D34" si="9">HEX2DEC(MID($B$1,$B4+0,1))</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E34" si="10">HEX2DEC(MID($B$1,$B4+1,1))</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <f>E4*255/15</f>
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="G4">
         <f>D4*255/15</f>
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="H4">
         <f>C4*255/15</f>
-        <v>0</v>
+        <v>238</v>
       </c>
       <c r="I4" t="str">
         <f>"  GGCOLOUR $"&amp;DEC2HEX(F4*65536+G4*256+H4,6)</f>
-        <v xml:space="preserve">  GGCOLOUR $444400</v>
+        <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
@@ -22488,7 +22489,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q4">
         <f t="shared" si="2"/>
@@ -22496,7 +22497,7 @@
       </c>
       <c r="R4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S4">
         <f t="shared" si="4"/>
@@ -22508,7 +22509,7 @@
       </c>
       <c r="U4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V4">
         <f t="shared" si="7"/>
@@ -22516,16 +22517,18 @@
       </c>
       <c r="W4" t="str">
         <f t="shared" ref="W4:W12" si="11">"  SMSCOLOUR $"&amp;DEC2HEX(T4*65536+U4*256+V4,6)</f>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-      <c r="AA4" t="str">
-        <f t="shared" ref="AA4:AA19" si="12">T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
       <c r="B5">
-        <f t="shared" ref="B5:B34" si="13">(ROW()-ROW($B$3))*6+1</f>
+        <f t="shared" ref="B5:B34" si="12">(ROW()-ROW($B$3))*6+1</f>
         <v>13</v>
       </c>
       <c r="C5">
@@ -22534,27 +22537,27 @@
       </c>
       <c r="D5">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F34" si="14">E5*255/15</f>
+        <f t="shared" ref="F5:F34" si="13">E5*255/15</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G22" si="14">D5*255/15</f>
         <v>136</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G22" si="15">D5*255/15</f>
-        <v>68</v>
-      </c>
       <c r="H5">
-        <f t="shared" ref="H5:H22" si="16">C5*255/15</f>
+        <f t="shared" ref="H5:H22" si="15">C5*255/15</f>
         <v>0</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I22" si="17">"  GGCOLOUR $"&amp;DEC2HEX(F5*65536+G5*256+H5,6)</f>
-        <v xml:space="preserve">  GGCOLOUR $884400</v>
+        <f t="shared" ref="I5:I22" si="16">"  GGCOLOUR $"&amp;DEC2HEX(F5*65536+G5*256+H5,6)</f>
+        <v xml:space="preserve">  GGCOLOUR $008800</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
@@ -22562,73 +22565,75 @@
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>238</v>
       </c>
       <c r="Q5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R5">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U5">
         <f t="shared" si="6"/>
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="V5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $005500</v>
-      </c>
-      <c r="AA5" t="str">
+        <v xml:space="preserve">  SMSCOLOUR $AAFFAA</v>
+      </c>
+      <c r="AA5">
+        <v>16</v>
+      </c>
+      <c r="AB5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B6">
         <f t="shared" si="12"/>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B6">
-        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="C6">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F6">
+        <f t="shared" si="13"/>
+        <v>136</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="14"/>
-        <v>238</v>
-      </c>
-      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="15"/>
-        <v>238</v>
-      </c>
-      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="16"/>
-        <v>238</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
+        <v xml:space="preserve">  GGCOLOUR $880000</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
@@ -22636,15 +22641,15 @@
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S6">
         <f t="shared" si="4"/>
@@ -22652,11 +22657,11 @@
       </c>
       <c r="T6">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U6">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="V6">
         <f t="shared" si="7"/>
@@ -22664,119 +22669,127 @@
       </c>
       <c r="W6" t="str">
         <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA6" t="str">
+        <f>T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
+        <v>0 85 0</v>
+      </c>
+      <c r="AB6" t="str">
+        <f>F3&amp;" "&amp;G3&amp;" "&amp;H3</f>
+        <v>68 0 136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B7">
         <f t="shared" si="12"/>
-        <v>0 85 0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B7">
-        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="C7">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="13"/>
+        <v>238</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="14"/>
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $EE4444</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA7" t="str">
+        <f>T4&amp;" "&amp;U4&amp;" "&amp;V4</f>
+        <v>0 170 0</v>
+      </c>
+      <c r="AB7" t="str">
+        <f t="shared" ref="AB7:AB21" si="17">F4&amp;" "&amp;G4&amp;" "&amp;H4</f>
+        <v>238 238 238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <f t="shared" si="12"/>
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="F7">
+      <c r="E8">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="13"/>
+        <v>238</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="14"/>
         <v>136</v>
       </c>
-      <c r="G7">
+      <c r="H8">
         <f t="shared" si="15"/>
-        <v>136</v>
-      </c>
-      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" si="16"/>
-        <v>136</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $888888</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="6"/>
-        <v>170</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W7" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="12"/>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B8">
-        <f t="shared" si="13"/>
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="10"/>
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="14"/>
-        <v>68</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="15"/>
-        <v>68</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="16"/>
-        <v>68</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $444444</v>
+        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
@@ -22815,338 +22828,358 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA8" t="str">
+        <f>T5&amp;" "&amp;U5&amp;" "&amp;V5</f>
+        <v>170 255 170</v>
+      </c>
+      <c r="AB8" t="str">
+        <f t="shared" si="17"/>
+        <v>0 136 0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B9">
         <f t="shared" si="12"/>
-        <v>0 170 0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B9">
-        <f t="shared" si="13"/>
         <v>37</v>
       </c>
       <c r="C9">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="14"/>
+        <v>68</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="15"/>
+        <v>238</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $4444EE</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="6"/>
+        <v>170</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+      </c>
+      <c r="AA9" t="str">
+        <f>T6&amp;" "&amp;U6&amp;" "&amp;V6</f>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="17"/>
+        <v>136 0 0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <f t="shared" si="12"/>
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA10" t="str">
+        <f>T7&amp;" "&amp;U7&amp;" "&amp;V7</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="17"/>
+        <v>238 68 68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <f t="shared" si="12"/>
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="13"/>
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="14"/>
+        <v>34</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="15"/>
+        <v>34</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $222222</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
+      </c>
+      <c r="AA11" t="str">
+        <f>T8&amp;" "&amp;U8&amp;" "&amp;V8</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="17"/>
+        <v>238 136 0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <f t="shared" si="12"/>
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="14"/>
+        <v>68</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="15"/>
+        <v>68</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve">  GGCOLOUR $444444</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+      <c r="AA12" t="str">
+        <f>T9&amp;" "&amp;U9&amp;" "&amp;V9</f>
+        <v>0 170 0</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="17"/>
+        <v>68 68 238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <f t="shared" si="12"/>
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="13"/>
+        <v>136</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="14"/>
         <v>136</v>
       </c>
-      <c r="G9">
+      <c r="H13">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H9">
+        <v>136</v>
+      </c>
+      <c r="I13" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $880000</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
-        <v>238</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="5"/>
-        <v>170</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="6"/>
-        <v>255</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="7"/>
-        <v>170</v>
-      </c>
-      <c r="W9" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $AAFFAA</v>
-      </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="12"/>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B10">
-        <f t="shared" si="13"/>
-        <v>43</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="15"/>
-        <v>68</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="16"/>
-        <v>136</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $004488</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="5"/>
-        <v>170</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="6"/>
-        <v>255</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="12"/>
-        <v>170 255 170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B11">
-        <f t="shared" si="13"/>
-        <v>49</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="1"/>
-        <v>136</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="6"/>
-        <v>170</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W11" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
-      </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="12"/>
-        <v>170 255 0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B12">
-        <f t="shared" si="13"/>
-        <v>55</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="6"/>
-        <v>170</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W12" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
-      </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="12"/>
-        <v>0 170 0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B13">
-        <f t="shared" si="13"/>
-        <v>61</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $888888</v>
       </c>
       <c r="O13">
         <f t="shared" ref="O13:O34" si="18">(ROW()-ROW($B$3))*3+1</f>
@@ -23154,15 +23187,15 @@
       </c>
       <c r="P13">
         <f t="shared" ref="P13:P34" si="19">HEX2DEC(MID($B$1,O13,2))</f>
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="Q13">
         <f t="shared" ref="Q13:Q34" si="20">_xlfn.BITAND(P13,3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R13">
         <f t="shared" ref="R13:R34" si="21">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S13">
         <f t="shared" ref="S13:S34" si="22">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
@@ -23170,11 +23203,11 @@
       </c>
       <c r="T13">
         <f t="shared" ref="T13:T34" si="23">Q13*255/3</f>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U13">
         <f t="shared" ref="U13:U34" si="24">R13*255/3</f>
-        <v>85</v>
+        <v>255</v>
       </c>
       <c r="V13">
         <f t="shared" ref="V13:V34" si="25">S13*255/3</f>
@@ -23182,16 +23215,20 @@
       </c>
       <c r="W13" t="str">
         <f t="shared" ref="W13:W34" si="26">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
-        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA13" t="str">
+        <f>T10&amp;" "&amp;U10&amp;" "&amp;V10</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="17"/>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B14">
         <f t="shared" si="12"/>
-        <v>0 170 0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B14">
-        <f t="shared" si="13"/>
         <v>67</v>
       </c>
       <c r="C14">
@@ -23200,27 +23237,27 @@
       </c>
       <c r="D14">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
+        <v>68</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H14">
+      <c r="I14" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $004400</v>
       </c>
       <c r="O14">
         <f t="shared" si="18"/>
@@ -23228,7 +23265,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="19"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <f t="shared" si="20"/>
@@ -23236,7 +23273,7 @@
       </c>
       <c r="R14">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14">
         <f t="shared" si="22"/>
@@ -23248,7 +23285,7 @@
       </c>
       <c r="U14">
         <f t="shared" si="24"/>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="V14">
         <f t="shared" si="25"/>
@@ -23256,16 +23293,20 @@
       </c>
       <c r="W14" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA14" t="str">
+        <f>T11&amp;" "&amp;U11&amp;" "&amp;V11</f>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="17"/>
+        <v>34 34 34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B15">
         <f t="shared" si="12"/>
-        <v>0 85 0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B15">
-        <f t="shared" si="13"/>
         <v>73</v>
       </c>
       <c r="C15">
@@ -23274,27 +23315,27 @@
       </c>
       <c r="D15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
+        <v>204</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H15">
+      <c r="I15" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $00CC00</v>
       </c>
       <c r="O15">
         <f t="shared" si="18"/>
@@ -23302,7 +23343,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="Q15">
         <f t="shared" si="20"/>
@@ -23310,7 +23351,7 @@
       </c>
       <c r="R15">
         <f t="shared" si="21"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S15">
         <f t="shared" si="22"/>
@@ -23322,7 +23363,7 @@
       </c>
       <c r="U15">
         <f t="shared" si="24"/>
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="V15">
         <f t="shared" si="25"/>
@@ -23330,16 +23371,20 @@
       </c>
       <c r="W15" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
       <c r="AA15" t="str">
+        <f>T12&amp;" "&amp;U12&amp;" "&amp;V12</f>
+        <v>0 85 0</v>
+      </c>
+      <c r="AB15" t="str">
+        <f t="shared" si="17"/>
+        <v>68 68 68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="B16">
         <f t="shared" si="12"/>
-        <v>0 85 0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="B16">
-        <f t="shared" si="13"/>
         <v>79</v>
       </c>
       <c r="C16">
@@ -23348,27 +23393,27 @@
       </c>
       <c r="D16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
+        <v>238</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H16">
+      <c r="I16" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $00EE00</v>
       </c>
       <c r="O16">
         <f t="shared" si="18"/>
@@ -23376,15 +23421,15 @@
       </c>
       <c r="P16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q16">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S16">
         <f t="shared" si="22"/>
@@ -23392,11 +23437,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U16">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="V16">
         <f t="shared" si="25"/>
@@ -23404,45 +23449,49 @@
       </c>
       <c r="W16" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA16" t="str">
+        <f>T13&amp;" "&amp;U13&amp;" "&amp;V13</f>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="17"/>
+        <v>136 136 136</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B17">
         <f t="shared" si="12"/>
-        <v>0 170 0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B17">
-        <f t="shared" si="13"/>
         <v>85</v>
       </c>
       <c r="C17">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F17">
+        <f t="shared" si="13"/>
+        <v>238</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
+        <v>170</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H17">
+        <v>170</v>
+      </c>
+      <c r="I17" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $EEAAAA</v>
       </c>
       <c r="O17">
         <f t="shared" si="18"/>
@@ -23450,7 +23499,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="19"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <f t="shared" si="20"/>
@@ -23481,13 +23530,17 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA17" t="str">
+        <f>T14&amp;" "&amp;U14&amp;" "&amp;V14</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="17"/>
+        <v>0 68 0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B18">
         <f t="shared" si="12"/>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B18">
-        <f t="shared" si="13"/>
         <v>91</v>
       </c>
       <c r="C18">
@@ -23503,19 +23556,19 @@
         <v>0</v>
       </c>
       <c r="F18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H18">
+      <c r="I18" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="17"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O18">
@@ -23524,7 +23577,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Q18">
         <f t="shared" si="20"/>
@@ -23532,7 +23585,7 @@
       </c>
       <c r="R18">
         <f t="shared" si="21"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <f t="shared" si="22"/>
@@ -23544,7 +23597,7 @@
       </c>
       <c r="U18">
         <f t="shared" si="24"/>
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="V18">
         <f t="shared" si="25"/>
@@ -23552,21 +23605,25 @@
       </c>
       <c r="W18" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA18" t="str">
+        <f>T15&amp;" "&amp;U15&amp;" "&amp;V15</f>
+        <v>0 85 0</v>
+      </c>
+      <c r="AB18" t="str">
+        <f t="shared" si="17"/>
+        <v>0 204 0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B19">
         <f t="shared" si="12"/>
-        <v>0 0 0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B19">
-        <f t="shared" si="13"/>
         <v>97</v>
       </c>
       <c r="C19">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <f t="shared" si="9"/>
@@ -23574,23 +23631,23 @@
       </c>
       <c r="E19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19">
+        <f t="shared" si="13"/>
+        <v>68</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H19">
+        <v>136</v>
+      </c>
+      <c r="I19" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $440088</v>
       </c>
       <c r="O19">
         <f t="shared" si="18"/>
@@ -23598,11 +23655,11 @@
       </c>
       <c r="P19">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="Q19">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19">
         <f t="shared" si="21"/>
@@ -23610,11 +23667,11 @@
       </c>
       <c r="S19">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T19">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U19">
         <f t="shared" si="24"/>
@@ -23622,49 +23679,53 @@
       </c>
       <c r="V19">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+        <v xml:space="preserve">  SMSCOLOUR $AA00AA</v>
       </c>
       <c r="AA19" t="str">
+        <f>T16&amp;" "&amp;U16&amp;" "&amp;V16</f>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB19" t="str">
+        <f t="shared" si="17"/>
+        <v>0 238 0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="B20">
         <f t="shared" si="12"/>
-        <v>0 170 0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.45">
-      <c r="B20">
-        <f t="shared" si="13"/>
         <v>103</v>
       </c>
       <c r="C20">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="F20">
+        <f t="shared" si="13"/>
+        <v>238</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="14"/>
         <v>238</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="15"/>
-        <v>68</v>
-      </c>
-      <c r="H20">
+        <v>238</v>
+      </c>
+      <c r="I20" t="str">
         <f t="shared" si="16"/>
-        <v>68</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $EE4444</v>
+        <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
       </c>
       <c r="O20">
         <f t="shared" si="18"/>
@@ -23672,11 +23733,11 @@
       </c>
       <c r="P20">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q20">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R20">
         <f t="shared" si="21"/>
@@ -23688,7 +23749,7 @@
       </c>
       <c r="T20">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U20">
         <f t="shared" si="24"/>
@@ -23700,12 +23761,20 @@
       </c>
       <c r="W20" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $AA0000</v>
+      </c>
+      <c r="AA20" t="str">
+        <f>T17&amp;" "&amp;U17&amp;" "&amp;V17</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB20" t="str">
+        <f t="shared" si="17"/>
+        <v>238 170 170</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>109</v>
       </c>
       <c r="C21">
@@ -23714,27 +23783,27 @@
       </c>
       <c r="D21">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F21">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="14"/>
-        <v>68</v>
-      </c>
-      <c r="G21">
+        <v>136</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="15"/>
-        <v>238</v>
-      </c>
-      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $44EE00</v>
+        <v xml:space="preserve">  GGCOLOUR $008800</v>
       </c>
       <c r="O21">
         <f t="shared" si="18"/>
@@ -23742,7 +23811,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="Q21">
         <f t="shared" si="20"/>
@@ -23750,7 +23819,7 @@
       </c>
       <c r="R21">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21">
         <f t="shared" si="22"/>
@@ -23762,7 +23831,7 @@
       </c>
       <c r="U21">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="V21">
         <f t="shared" si="25"/>
@@ -23770,12 +23839,20 @@
       </c>
       <c r="W21" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+      <c r="AA21" t="str">
+        <f>T18&amp;" "&amp;U18&amp;" "&amp;V18</f>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB21" t="str">
+        <f t="shared" si="17"/>
+        <v>0 0 0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>115</v>
       </c>
       <c r="C22">
@@ -23788,23 +23865,23 @@
       </c>
       <c r="E22">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F22">
+        <f t="shared" si="13"/>
+        <v>136</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H22">
+      <c r="I22" t="str">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I22" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
+        <v xml:space="preserve">  GGCOLOUR $880000</v>
       </c>
       <c r="O22">
         <f t="shared" si="18"/>
@@ -23812,7 +23889,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q22">
         <f t="shared" si="20"/>
@@ -23820,7 +23897,7 @@
       </c>
       <c r="R22">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22">
         <f t="shared" si="22"/>
@@ -23832,7 +23909,7 @@
       </c>
       <c r="U22">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="V22">
         <f t="shared" si="25"/>
@@ -23840,41 +23917,41 @@
       </c>
       <c r="W22" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>121</v>
       </c>
       <c r="C23">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F23">
-        <f t="shared" si="14"/>
-        <v>68</v>
+        <f t="shared" si="13"/>
+        <v>238</v>
       </c>
       <c r="G23">
         <f t="shared" ref="G23:G34" si="27">D23*255/15</f>
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="H23">
         <f t="shared" ref="H23:H34" si="28">C23*255/15</f>
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" ref="I23:I34" si="29">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
-        <v xml:space="preserve">  GGCOLOUR $4488EE</v>
+        <v xml:space="preserve">  GGCOLOUR $EE4444</v>
       </c>
       <c r="O23">
         <f t="shared" si="18"/>
@@ -23882,7 +23959,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="Q23">
         <f t="shared" si="20"/>
@@ -23890,7 +23967,7 @@
       </c>
       <c r="R23">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S23">
         <f t="shared" si="22"/>
@@ -23902,7 +23979,7 @@
       </c>
       <c r="U23">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V23">
         <f t="shared" si="25"/>
@@ -23910,41 +23987,41 @@
       </c>
       <c r="W23" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>127</v>
       </c>
       <c r="C24">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F24">
-        <f t="shared" si="14"/>
-        <v>68</v>
+        <f t="shared" si="13"/>
+        <v>238</v>
       </c>
       <c r="G24">
         <f t="shared" si="27"/>
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="H24">
         <f t="shared" si="28"/>
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $444444</v>
+        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
       </c>
       <c r="O24">
         <f t="shared" si="18"/>
@@ -23952,7 +24029,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q24">
         <f t="shared" si="20"/>
@@ -23960,7 +24037,7 @@
       </c>
       <c r="R24">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S24">
         <f t="shared" si="22"/>
@@ -23972,7 +24049,7 @@
       </c>
       <c r="U24">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V24">
         <f t="shared" si="25"/>
@@ -23980,17 +24057,17 @@
       </c>
       <c r="W24" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>133</v>
       </c>
       <c r="C25">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <f t="shared" si="9"/>
@@ -24001,7 +24078,7 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>136</v>
       </c>
       <c r="G25">
@@ -24010,11 +24087,11 @@
       </c>
       <c r="H25">
         <f t="shared" si="28"/>
-        <v>136</v>
+        <v>238</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $888888</v>
+        <v xml:space="preserve">  GGCOLOUR $8888EE</v>
       </c>
       <c r="O25">
         <f t="shared" si="18"/>
@@ -24022,7 +24099,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="Q25">
         <f t="shared" si="20"/>
@@ -24053,38 +24130,38 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>139</v>
       </c>
       <c r="C26">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <f t="shared" si="9"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <f t="shared" si="14"/>
-        <v>238</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="G26">
         <f t="shared" si="27"/>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <f t="shared" si="28"/>
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O26">
         <f t="shared" si="18"/>
@@ -24123,9 +24200,9 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>145</v>
       </c>
       <c r="C27">
@@ -24134,19 +24211,19 @@
       </c>
       <c r="D27">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <f t="shared" si="14"/>
-        <v>238</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="G27">
         <f t="shared" si="27"/>
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <f t="shared" si="28"/>
@@ -24154,7 +24231,7 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O27">
         <f t="shared" si="18"/>
@@ -24162,7 +24239,7 @@
       </c>
       <c r="P27">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>192</v>
       </c>
       <c r="Q27">
         <f t="shared" si="20"/>
@@ -24193,9 +24270,9 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>151</v>
       </c>
       <c r="C28">
@@ -24211,7 +24288,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G28">
@@ -24263,9 +24340,9 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>157</v>
       </c>
       <c r="C29">
@@ -24281,7 +24358,7 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G29">
@@ -24302,7 +24379,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>224</v>
       </c>
       <c r="Q29">
         <f t="shared" si="20"/>
@@ -24314,7 +24391,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T29">
         <f t="shared" si="23"/>
@@ -24326,16 +24403,16 @@
       </c>
       <c r="V29">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="W29" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $0000AA</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>163</v>
       </c>
       <c r="C30">
@@ -24351,7 +24428,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G30">
@@ -24403,9 +24480,9 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>169</v>
       </c>
       <c r="C31">
@@ -24421,7 +24498,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G31">
@@ -24442,40 +24519,40 @@
       </c>
       <c r="P31">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="Q31">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R31">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S31">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T31">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U31">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="V31">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="W31" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  SMSCOLOUR $AAFFAA</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>175</v>
       </c>
       <c r="C32">
@@ -24491,7 +24568,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G32">
@@ -24512,15 +24589,15 @@
       </c>
       <c r="P32">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q32">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R32">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S32">
         <f t="shared" si="22"/>
@@ -24528,11 +24605,11 @@
       </c>
       <c r="T32">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="U32">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V32">
         <f t="shared" si="25"/>
@@ -24540,12 +24617,12 @@
       </c>
       <c r="W32" t="str">
         <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+        <v xml:space="preserve">  SMSCOLOUR $AAAA00</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>181</v>
       </c>
       <c r="C33">
@@ -24561,7 +24638,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G33">
@@ -24615,7 +24692,7 @@
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.45">
       <c r="B34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>187</v>
       </c>
       <c r="C34">
@@ -24631,7 +24708,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G34">

</xml_diff>

<commit_message>
Variable(s) used for timers in menus
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxim\Documents\Code\C#\MicroMachinesEditor\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxim 2\Documents\Code\C#\MicroMachinesEditor\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9765" windowHeight="9195" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="9765" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Splash sound" sheetId="2" r:id="rId2"/>
     <sheet name="Splash tile data" sheetId="3" r:id="rId3"/>
     <sheet name="Palette" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="190">
   <si>
     <t>0f0e0f0e0d0e0e0f</t>
   </si>
@@ -468,6 +468,132 @@
   <si>
     <t>04 08 EE 0E 80 00 08 00 4E 04 8E 00 44 0E 00 00 22 02 44 04 88 08 40 00 C0 00 E0 00 AE 0A 00 00 04 08 EE 0E 80 00 08 00 4E 04 8E 00 88 0E 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00 00</t>
   </si>
+  <si>
+    <t>00c8</t>
+  </si>
+  <si>
+    <t>01ac</t>
+  </si>
+  <si>
+    <t>046C</t>
+  </si>
+  <si>
+    <t>083A</t>
+  </si>
+  <si>
+    <t>0A0C</t>
+  </si>
+  <si>
+    <t>0AF0</t>
+  </si>
+  <si>
+    <t>0BDA</t>
+  </si>
+  <si>
+    <t>0CC4</t>
+  </si>
+  <si>
+    <t>0DC0</t>
+  </si>
+  <si>
+    <t>0F6C</t>
+  </si>
+  <si>
+    <t>13F6</t>
+  </si>
+  <si>
+    <t>14F0</t>
+  </si>
+  <si>
+    <t>15DE</t>
+  </si>
+  <si>
+    <t>16C2</t>
+  </si>
+  <si>
+    <t>178E</t>
+  </si>
+  <si>
+    <t>185E</t>
+  </si>
+  <si>
+    <t>1A34</t>
+  </si>
+  <si>
+    <t>1B24</t>
+  </si>
+  <si>
+    <t>1C1E</t>
+  </si>
+  <si>
+    <t>1C2A</t>
+  </si>
+  <si>
+    <t>1D16</t>
+  </si>
+  <si>
+    <t>1EE8</t>
+  </si>
+  <si>
+    <t>1FD4</t>
+  </si>
+  <si>
+    <t>20C8</t>
+  </si>
+  <si>
+    <t>21B4</t>
+  </si>
+  <si>
+    <t>223B</t>
+  </si>
+  <si>
+    <t>22C2</t>
+  </si>
+  <si>
+    <t>23AE</t>
+  </si>
+  <si>
+    <t>0e88</t>
+  </si>
+  <si>
+    <t>1e02</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>RAM code addresses</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>3b97d</t>
+  </si>
+  <si>
+    <t>Dest</t>
+  </si>
+  <si>
+    <t>d7bd</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>db2f</t>
+  </si>
+  <si>
+    <t>hex</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>s @ 50Hz</t>
+  </si>
+  <si>
+    <t>s @ 60Hz</t>
+  </si>
 </sst>
 </file>
 
@@ -509,11 +635,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,11 +1098,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="512945704"/>
-        <c:axId val="512941784"/>
+        <c:axId val="406183536"/>
+        <c:axId val="406184320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="512945704"/>
+        <c:axId val="406183536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="512941784"/>
+        <c:crossAx val="406184320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512941784"/>
+        <c:axId val="406184320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1077,7 +1204,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="512945704"/>
+        <c:crossAx val="406183536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1499,11 +1626,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="512948056"/>
-        <c:axId val="512942568"/>
+        <c:axId val="406181184"/>
+        <c:axId val="406185104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="512948056"/>
+        <c:axId val="406181184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +1672,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="512942568"/>
+        <c:crossAx val="406185104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +1680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512942568"/>
+        <c:axId val="406185104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1731,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="512948056"/>
+        <c:crossAx val="406181184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3117,10 +3244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF52"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46:P53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5665,7 +5792,7 @@
         <v>6A</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>22</v>
       </c>
@@ -5705,7 +5832,7 @@
         <v>A9</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>23</v>
       </c>
@@ -5742,7 +5869,7 @@
         <v>1296A</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>4</v>
       </c>
@@ -5766,6 +5893,85 @@
       </c>
       <c r="K52" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" t="str">
+        <f>DEC2HEX(HEX2DEC(A58)+HEX2DEC(B55)-HEX2DEC(B56))</f>
+        <v>3BCEF</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62">
+        <f>HEX2DEC(B61)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63">
+        <f>B62/50</f>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>189</v>
+      </c>
+      <c r="B64">
+        <f>B62/60</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B65" t="str">
+        <f>B63&amp;"s @ 50Hz, "&amp;B64&amp;"s @ 60Hz"</f>
+        <v>1.92s @ 50Hz, 1.6s @ 60Hz</v>
       </c>
     </row>
   </sheetData>
@@ -22294,7 +22500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -22672,7 +22878,7 @@
         <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA6" t="str">
-        <f>T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
+        <f t="shared" ref="AA6:AA21" si="17">T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
         <v>0 85 0</v>
       </c>
       <c r="AB6" t="str">
@@ -22750,11 +22956,11 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA7" t="str">
-        <f>T4&amp;" "&amp;U4&amp;" "&amp;V4</f>
+        <f t="shared" si="17"/>
         <v>0 170 0</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" ref="AB7:AB21" si="17">F4&amp;" "&amp;G4&amp;" "&amp;H4</f>
+        <f t="shared" ref="AB7:AB21" si="18">F4&amp;" "&amp;G4&amp;" "&amp;H4</f>
         <v>238 238 238</v>
       </c>
     </row>
@@ -22828,11 +23034,11 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA8" t="str">
-        <f>T5&amp;" "&amp;U5&amp;" "&amp;V5</f>
+        <f t="shared" si="17"/>
         <v>170 255 170</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0 136 0</v>
       </c>
     </row>
@@ -22906,11 +23112,11 @@
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
       <c r="AA9" t="str">
-        <f>T6&amp;" "&amp;U6&amp;" "&amp;V6</f>
+        <f t="shared" si="17"/>
         <v>170 255 0</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>136 0 0</v>
       </c>
     </row>
@@ -22984,11 +23190,11 @@
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
       <c r="AA10" t="str">
-        <f>T7&amp;" "&amp;U7&amp;" "&amp;V7</f>
+        <f t="shared" si="17"/>
         <v>0 0 0</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>238 68 68</v>
       </c>
     </row>
@@ -23062,11 +23268,11 @@
         <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA11" t="str">
-        <f>T8&amp;" "&amp;U8&amp;" "&amp;V8</f>
+        <f t="shared" si="17"/>
         <v>0 0 0</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>238 136 0</v>
       </c>
     </row>
@@ -23140,11 +23346,11 @@
         <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
       <c r="AA12" t="str">
-        <f>T9&amp;" "&amp;U9&amp;" "&amp;V9</f>
+        <f t="shared" si="17"/>
         <v>0 170 0</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>68 68 238</v>
       </c>
     </row>
@@ -23182,47 +23388,47 @@
         <v xml:space="preserve">  GGCOLOUR $888888</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O34" si="18">(ROW()-ROW($B$3))*3+1</f>
+        <f t="shared" ref="O13:O34" si="19">(ROW()-ROW($B$3))*3+1</f>
         <v>31</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P34" si="19">HEX2DEC(MID($B$1,O13,2))</f>
+        <f t="shared" ref="P13:P34" si="20">HEX2DEC(MID($B$1,O13,2))</f>
         <v>142</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13:Q34" si="20">_xlfn.BITAND(P13,3)</f>
+        <f t="shared" ref="Q13:Q34" si="21">_xlfn.BITAND(P13,3)</f>
         <v>2</v>
       </c>
       <c r="R13">
-        <f t="shared" ref="R13:R34" si="21">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
+        <f t="shared" ref="R13:R34" si="22">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,2),3)</f>
         <v>3</v>
       </c>
       <c r="S13">
-        <f t="shared" ref="S13:S34" si="22">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
+        <f t="shared" ref="S13:S34" si="23">_xlfn.BITAND(_xlfn.BITRSHIFT(P13,4),3)</f>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13:T34" si="23">Q13*255/3</f>
+        <f t="shared" ref="T13:T34" si="24">Q13*255/3</f>
         <v>170</v>
       </c>
       <c r="U13">
-        <f t="shared" ref="U13:U34" si="24">R13*255/3</f>
+        <f t="shared" ref="U13:U34" si="25">R13*255/3</f>
         <v>255</v>
       </c>
       <c r="V13">
-        <f t="shared" ref="V13:V34" si="25">S13*255/3</f>
+        <f t="shared" ref="V13:V34" si="26">S13*255/3</f>
         <v>0</v>
       </c>
       <c r="W13" t="str">
-        <f t="shared" ref="W13:W34" si="26">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
+        <f t="shared" ref="W13:W34" si="27">"  SMSCOLOUR $"&amp;DEC2HEX(T13*65536+U13*256+V13,6)</f>
         <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
       </c>
       <c r="AA13" t="str">
-        <f>T10&amp;" "&amp;U10&amp;" "&amp;V10</f>
+        <f t="shared" si="17"/>
         <v>0 0 0</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0 0 0</v>
       </c>
     </row>
@@ -23260,47 +23466,47 @@
         <v xml:space="preserve">  GGCOLOUR $004400</v>
       </c>
       <c r="O14">
+        <f t="shared" si="19"/>
+        <v>34</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="17"/>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB14" t="str">
         <f t="shared" si="18"/>
-        <v>34</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W14" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-      <c r="AA14" t="str">
-        <f>T11&amp;" "&amp;U11&amp;" "&amp;V11</f>
-        <v>170 255 0</v>
-      </c>
-      <c r="AB14" t="str">
-        <f t="shared" si="17"/>
         <v>34 34 34</v>
       </c>
     </row>
@@ -23338,47 +23544,47 @@
         <v xml:space="preserve">  GGCOLOUR $00CC00</v>
       </c>
       <c r="O15">
+        <f t="shared" si="19"/>
+        <v>37</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="20"/>
+        <v>68</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="25"/>
+        <v>85</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W15" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+      <c r="AA15" t="str">
+        <f t="shared" si="17"/>
+        <v>0 85 0</v>
+      </c>
+      <c r="AB15" t="str">
         <f t="shared" si="18"/>
-        <v>37</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="19"/>
-        <v>68</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="24"/>
-        <v>85</v>
-      </c>
-      <c r="V15">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W15" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $005500</v>
-      </c>
-      <c r="AA15" t="str">
-        <f>T12&amp;" "&amp;U12&amp;" "&amp;V12</f>
-        <v>0 85 0</v>
-      </c>
-      <c r="AB15" t="str">
-        <f t="shared" si="17"/>
         <v>68 68 68</v>
       </c>
     </row>
@@ -23416,47 +23622,47 @@
         <v xml:space="preserve">  GGCOLOUR $00EE00</v>
       </c>
       <c r="O16">
+        <f t="shared" si="19"/>
+        <v>40</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="20"/>
+        <v>14</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="24"/>
+        <v>170</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="25"/>
+        <v>255</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="17"/>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB16" t="str">
         <f t="shared" si="18"/>
-        <v>40</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="19"/>
-        <v>14</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="R16">
-        <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="23"/>
-        <v>170</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="24"/>
-        <v>255</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W16" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $AAFF00</v>
-      </c>
-      <c r="AA16" t="str">
-        <f>T13&amp;" "&amp;U13&amp;" "&amp;V13</f>
-        <v>170 255 0</v>
-      </c>
-      <c r="AB16" t="str">
-        <f t="shared" si="17"/>
         <v>136 136 136</v>
       </c>
     </row>
@@ -23494,47 +23700,47 @@
         <v xml:space="preserve">  GGCOLOUR $EEAAAA</v>
       </c>
       <c r="O17">
+        <f t="shared" si="19"/>
+        <v>43</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="17"/>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB17" t="str">
         <f t="shared" si="18"/>
-        <v>43</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W17" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-      <c r="AA17" t="str">
-        <f>T14&amp;" "&amp;U14&amp;" "&amp;V14</f>
-        <v>0 0 0</v>
-      </c>
-      <c r="AB17" t="str">
-        <f t="shared" si="17"/>
         <v>0 68 0</v>
       </c>
     </row>
@@ -23572,47 +23778,47 @@
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O18">
+        <f t="shared" si="19"/>
+        <v>46</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W18" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+      <c r="AA18" t="str">
+        <f t="shared" si="17"/>
+        <v>0 85 0</v>
+      </c>
+      <c r="AB18" t="str">
         <f t="shared" si="18"/>
-        <v>46</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W18" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $000000</v>
-      </c>
-      <c r="AA18" t="str">
-        <f>T15&amp;" "&amp;U15&amp;" "&amp;V15</f>
-        <v>0 85 0</v>
-      </c>
-      <c r="AB18" t="str">
-        <f t="shared" si="17"/>
         <v>0 204 0</v>
       </c>
     </row>
@@ -23650,47 +23856,47 @@
         <v xml:space="preserve">  GGCOLOUR $440088</v>
       </c>
       <c r="O19">
+        <f t="shared" si="19"/>
+        <v>49</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="20"/>
+        <v>34</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="24"/>
+        <v>170</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $AA00AA</v>
+      </c>
+      <c r="AA19" t="str">
+        <f t="shared" si="17"/>
+        <v>170 255 0</v>
+      </c>
+      <c r="AB19" t="str">
         <f t="shared" si="18"/>
-        <v>49</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="19"/>
-        <v>34</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="R19">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="23"/>
-        <v>170</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <f t="shared" si="25"/>
-        <v>170</v>
-      </c>
-      <c r="W19" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $AA00AA</v>
-      </c>
-      <c r="AA19" t="str">
-        <f>T16&amp;" "&amp;U16&amp;" "&amp;V16</f>
-        <v>170 255 0</v>
-      </c>
-      <c r="AB19" t="str">
-        <f t="shared" si="17"/>
         <v>0 238 0</v>
       </c>
     </row>
@@ -23728,47 +23934,47 @@
         <v xml:space="preserve">  GGCOLOUR $EEEEEE</v>
       </c>
       <c r="O20">
+        <f t="shared" si="19"/>
+        <v>52</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="24"/>
+        <v>170</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W20" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $AA0000</v>
+      </c>
+      <c r="AA20" t="str">
+        <f t="shared" si="17"/>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB20" t="str">
         <f t="shared" si="18"/>
-        <v>52</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <f t="shared" si="23"/>
-        <v>170</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W20" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $AA0000</v>
-      </c>
-      <c r="AA20" t="str">
-        <f>T17&amp;" "&amp;U17&amp;" "&amp;V17</f>
-        <v>0 0 0</v>
-      </c>
-      <c r="AB20" t="str">
-        <f t="shared" si="17"/>
         <v>238 170 170</v>
       </c>
     </row>
@@ -23806,47 +24012,47 @@
         <v xml:space="preserve">  GGCOLOUR $008800</v>
       </c>
       <c r="O21">
+        <f t="shared" si="19"/>
+        <v>55</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="20"/>
+        <v>68</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="25"/>
+        <v>85</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W21" t="str">
+        <f t="shared" si="27"/>
+        <v xml:space="preserve">  SMSCOLOUR $005500</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" si="17"/>
+        <v>0 0 0</v>
+      </c>
+      <c r="AB21" t="str">
         <f t="shared" si="18"/>
-        <v>55</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="19"/>
-        <v>68</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="24"/>
-        <v>85</v>
-      </c>
-      <c r="V21">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W21" t="str">
-        <f t="shared" si="26"/>
-        <v xml:space="preserve">  SMSCOLOUR $005500</v>
-      </c>
-      <c r="AA21" t="str">
-        <f>T18&amp;" "&amp;U18&amp;" "&amp;V18</f>
-        <v>0 0 0</v>
-      </c>
-      <c r="AB21" t="str">
-        <f t="shared" si="17"/>
         <v>0 0 0</v>
       </c>
     </row>
@@ -23884,39 +24090,39 @@
         <v xml:space="preserve">  GGCOLOUR $880000</v>
       </c>
       <c r="O22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>58</v>
       </c>
       <c r="P22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="S22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="T22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="U22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>85</v>
       </c>
       <c r="V22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W22" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">  SMSCOLOUR $005500</v>
       </c>
     </row>
@@ -23942,51 +24148,51 @@
         <v>238</v>
       </c>
       <c r="G23">
-        <f t="shared" ref="G23:G34" si="27">D23*255/15</f>
+        <f t="shared" ref="G23:G34" si="28">D23*255/15</f>
         <v>68</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H34" si="28">C23*255/15</f>
+        <f t="shared" ref="H23:H34" si="29">C23*255/15</f>
         <v>68</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23:I34" si="29">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
+        <f t="shared" ref="I23:I34" si="30">"  GGCOLOUR $"&amp;DEC2HEX(F23*65536+G23*256+H23,6)</f>
         <v xml:space="preserve">  GGCOLOUR $EE4444</v>
       </c>
       <c r="O23">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>61</v>
       </c>
       <c r="P23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>136</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="S23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="T23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="U23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>170</v>
       </c>
       <c r="V23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W23" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
     </row>
@@ -24012,51 +24218,51 @@
         <v>238</v>
       </c>
       <c r="G24">
+        <f t="shared" si="28"/>
+        <v>136</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="19"/>
+        <v>64</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="25"/>
+        <v>170</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W24" t="str">
         <f t="shared" si="27"/>
-        <v>136</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $EE8800</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="18"/>
-        <v>64</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="19"/>
-        <v>8</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="24"/>
-        <v>170</v>
-      </c>
-      <c r="V24">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W24" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $00AA00</v>
       </c>
     </row>
@@ -24082,51 +24288,51 @@
         <v>136</v>
       </c>
       <c r="G25">
+        <f t="shared" si="28"/>
+        <v>136</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="29"/>
+        <v>238</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $8888EE</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="19"/>
+        <v>67</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="20"/>
+        <v>64</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W25" t="str">
         <f t="shared" si="27"/>
-        <v>136</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="28"/>
-        <v>238</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $8888EE</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="18"/>
-        <v>67</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="19"/>
-        <v>64</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V25">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W25" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24152,51 +24358,51 @@
         <v>0</v>
       </c>
       <c r="G26">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="19"/>
+        <v>70</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W26" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="18"/>
-        <v>70</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W26" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24222,51 +24428,51 @@
         <v>0</v>
       </c>
       <c r="G27">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="19"/>
+        <v>73</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="20"/>
+        <v>192</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W27" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="18"/>
-        <v>73</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="19"/>
-        <v>192</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W27" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24292,51 +24498,51 @@
         <v>0</v>
       </c>
       <c r="G28">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="19"/>
+        <v>76</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W28" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="18"/>
-        <v>76</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T28">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V28">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W28" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24362,51 +24568,51 @@
         <v>0</v>
       </c>
       <c r="G29">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="19"/>
+        <v>79</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="20"/>
+        <v>224</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="W29" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="18"/>
-        <v>79</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="19"/>
-        <v>224</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <f t="shared" si="25"/>
-        <v>170</v>
-      </c>
-      <c r="W29" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $0000AA</v>
       </c>
     </row>
@@ -24432,51 +24638,51 @@
         <v>0</v>
       </c>
       <c r="G30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="19"/>
+        <v>82</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W30" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="18"/>
-        <v>82</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T30">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V30">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W30" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24502,51 +24708,51 @@
         <v>0</v>
       </c>
       <c r="G31">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="19"/>
+        <v>85</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="20"/>
+        <v>174</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="24"/>
+        <v>170</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="25"/>
+        <v>255</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="W31" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="18"/>
-        <v>85</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="19"/>
-        <v>174</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="23"/>
-        <v>170</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="24"/>
-        <v>255</v>
-      </c>
-      <c r="V31">
-        <f t="shared" si="25"/>
-        <v>170</v>
-      </c>
-      <c r="W31" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $AAFFAA</v>
       </c>
     </row>
@@ -24572,51 +24778,51 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v xml:space="preserve">  GGCOLOUR $000000</v>
       </c>
       <c r="O32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>88</v>
       </c>
       <c r="P32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="R32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="S32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="T32">
-        <f t="shared" si="23"/>
-        <v>170</v>
-      </c>
-      <c r="U32">
         <f t="shared" si="24"/>
         <v>170</v>
       </c>
+      <c r="U32">
+        <f t="shared" si="25"/>
+        <v>170</v>
+      </c>
       <c r="V32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="W32" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v xml:space="preserve">  SMSCOLOUR $AAAA00</v>
       </c>
     </row>
@@ -24642,51 +24848,51 @@
         <v>0</v>
       </c>
       <c r="G33">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="19"/>
+        <v>91</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W33" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="18"/>
-        <v>91</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W33" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
       </c>
     </row>
@@ -24712,52 +24918,957 @@
         <v>0</v>
       </c>
       <c r="G34">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="30"/>
+        <v xml:space="preserve">  GGCOLOUR $000000</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="19"/>
+        <v>94</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W34" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="I34" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">  GGCOLOUR $000000</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="18"/>
-        <v>94</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="U34">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="V34">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="W34" t="str">
-        <f t="shared" si="26"/>
         <v xml:space="preserve">  SMSCOLOUR $000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <f>HEX2DEC(A2)</f>
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>200</v>
+      </c>
+      <c r="D2" t="str">
+        <f>DEC2HEX(C2)</f>
+        <v>C8</v>
+      </c>
+      <c r="E2" t="str">
+        <f>DEC2HEX(202085+B1)</f>
+        <v>31565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B43" si="0">HEX2DEC(A3)</f>
+        <v>428</v>
+      </c>
+      <c r="C3">
+        <f>B3-B2</f>
+        <v>228</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D43" si="1">DEC2HEX(C3)</f>
+        <v>E4</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E43" si="2">DEC2HEX(202085+B2)</f>
+        <v>3162D</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>294</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C43" si="3">B4-B3</f>
+        <v>232</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>E8</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>31711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>382</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>898</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>317F9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1132</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>318E7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>568</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1384</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>252</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>FC</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>319D1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>652</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1618</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>31ACD</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>748</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1864</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>246</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>F6</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>31BB7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2106</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>242</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>F2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>31CAD</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>928</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>2344</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>31D9F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>2572</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>31E8D</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>31F71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>3034</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>32055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>3268</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>3213F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>3520</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>252</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>FC</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>32229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>3720</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>C8</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>32325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>3948</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>323ED</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>1050</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4176</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>324D1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>1134</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4404</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>325B5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>1222</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4642</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>32699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>1306</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4870</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>32787</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5110</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>F0</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>3286B</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5360</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>FA</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>3295B</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5598</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>32A55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>5826</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>32B43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>6030</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>CC</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>32C27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>6238</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>D0</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>32CF3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>1946</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>6470</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>E8</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>32DC3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>6708</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>32EAB</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>6948</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>F0</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>32F99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>7198</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>FA</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>33089</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>7210</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>33183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>7446</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>3318F</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>7682</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>3327B</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>7912</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>33367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>8148</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>3344D</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>8392</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>F4</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>33539</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>8628</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>3362D</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>8763</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>33719</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>8898</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>337A0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>9134</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v>33827</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>2498</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>9368</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>33913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More assets removed, code improvements, macros, data blobs split up a bit
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="9765" windowHeight="9195"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="7425" windowHeight="3743"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="192">
   <si>
     <t>0f0e0f0e0d0e0e0f</t>
   </si>
@@ -594,6 +595,12 @@
   <si>
     <t>s @ 60Hz</t>
   </si>
+  <si>
+    <t>s @ 25Hz</t>
+  </si>
+  <si>
+    <t>s @ 30Hz</t>
+  </si>
 </sst>
 </file>
 
@@ -1098,11 +1105,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="406183536"/>
-        <c:axId val="406184320"/>
+        <c:axId val="434820616"/>
+        <c:axId val="434821400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="406183536"/>
+        <c:axId val="434820616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406184320"/>
+        <c:crossAx val="434821400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1152,7 +1159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="406184320"/>
+        <c:axId val="434821400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1204,7 +1211,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406183536"/>
+        <c:crossAx val="434820616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1626,11 +1633,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="406181184"/>
-        <c:axId val="406185104"/>
+        <c:axId val="453813144"/>
+        <c:axId val="453817456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="406181184"/>
+        <c:axId val="453813144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1679,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406185104"/>
+        <c:crossAx val="453817456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1680,7 +1687,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="406185104"/>
+        <c:axId val="453817456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="406181184"/>
+        <c:crossAx val="453813144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3244,10 +3251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF65"/>
+  <dimension ref="A1:AF73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5933,12 +5940,33 @@
         <v>3BCEF</v>
       </c>
     </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>186</v>
       </c>
       <c r="B61">
-        <v>60</v>
+        <v>86</v>
+      </c>
+      <c r="E61">
+        <v>11</v>
+      </c>
+      <c r="F61" t="str">
+        <f>DEC2HEX(E61)</f>
+        <v>B</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.45">
@@ -5947,7 +5975,14 @@
       </c>
       <c r="B62">
         <f>HEX2DEC(B61)</f>
-        <v>96</v>
+        <v>134</v>
+      </c>
+      <c r="E62">
+        <v>24</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" ref="F62:F73" si="15">DEC2HEX(E62)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
@@ -5956,7 +5991,14 @@
       </c>
       <c r="B63">
         <f>B62/50</f>
-        <v>1.92</v>
+        <v>2.68</v>
+      </c>
+      <c r="E63">
+        <v>27</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="15"/>
+        <v>1B</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
@@ -5965,13 +6007,117 @@
       </c>
       <c r="B64">
         <f>B62/60</f>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
+        <v>2.2333333333333334</v>
+      </c>
+      <c r="E64">
+        <v>107</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="15"/>
+        <v>6B</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B65" t="str">
         <f>B63&amp;"s @ 50Hz, "&amp;B64&amp;"s @ 60Hz"</f>
-        <v>1.92s @ 50Hz, 1.6s @ 60Hz</v>
+        <v>2.68s @ 50Hz, 2.23333333333333s @ 60Hz</v>
+      </c>
+      <c r="E65">
+        <v>120</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="15"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66">
+        <f>B62/25</f>
+        <v>5.36</v>
+      </c>
+      <c r="E66">
+        <v>123</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="15"/>
+        <v>7B</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67">
+        <f>B62/30</f>
+        <v>4.4666666666666668</v>
+      </c>
+      <c r="E67">
+        <v>136</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="15"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B68" t="str">
+        <f>B66&amp;"s @ 50Hz, "&amp;B67&amp;"s @ 60Hz (half rate)"</f>
+        <v>5.36s @ 50Hz, 4.46666666666667s @ 60Hz (half rate)</v>
+      </c>
+      <c r="E68">
+        <v>139</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="15"/>
+        <v>8B</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E69">
+        <v>152</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="15"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E70">
+        <v>155</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="15"/>
+        <v>9B</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E71">
+        <v>232</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="15"/>
+        <v>E8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E72">
+        <v>235</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="15"/>
+        <v>EB</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E73">
+        <v>249</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="15"/>
+        <v>F9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of stuff, I'm not keeping track well
</commit_message>
<xml_diff>
--- a/Analysis/Micro Machines tables.xlsx
+++ b/Analysis/Micro Machines tables.xlsx
@@ -9,17 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="7425" windowHeight="3743" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="7425" windowHeight="3743" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Splash sound" sheetId="2" r:id="rId2"/>
-    <sheet name="Splash tile data" sheetId="3" r:id="rId3"/>
-    <sheet name="Palette" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId3"/>
+    <sheet name="Splash tile data" sheetId="3" r:id="rId4"/>
+    <sheet name="Palette" sheetId="4" r:id="rId5"/>
     <sheet name="SFX tone graphs" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1141,11 +1144,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="37966776"/>
-        <c:axId val="37962856"/>
+        <c:axId val="448293376"/>
+        <c:axId val="239165080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37966776"/>
+        <c:axId val="448293376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1190,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37962856"/>
+        <c:crossAx val="239165080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1195,7 +1198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37962856"/>
+        <c:axId val="239165080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1247,7 +1250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37966776"/>
+        <c:crossAx val="448293376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1311,6 +1314,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1669,11 +1673,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="37963640"/>
-        <c:axId val="37964816"/>
+        <c:axId val="239168216"/>
+        <c:axId val="447076112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37963640"/>
+        <c:axId val="239168216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1719,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37964816"/>
+        <c:crossAx val="447076112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1723,7 +1727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37964816"/>
+        <c:axId val="447076112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1774,7 +1778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37963640"/>
+        <c:crossAx val="239168216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4049,11 +4053,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="466150032"/>
-        <c:axId val="466148856"/>
+        <c:axId val="447071800"/>
+        <c:axId val="238227064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="466150032"/>
+        <c:axId val="447071800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4095,7 +4099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466148856"/>
+        <c:crossAx val="238227064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4103,7 +4107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="466148856"/>
+        <c:axId val="238227064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4154,7 +4158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466150032"/>
+        <c:crossAx val="447071800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11539,6 +11543,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y152"/>
   <sheetViews>
     <sheetView topLeftCell="B99" workbookViewId="0">
@@ -25764,7 +25780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB34"/>
   <sheetViews>
@@ -28239,914 +28255,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2">
-        <f>HEX2DEC(A2)</f>
-        <v>200</v>
-      </c>
-      <c r="C2">
-        <f>B2</f>
-        <v>200</v>
-      </c>
-      <c r="D2" t="str">
-        <f>DEC2HEX(C2)</f>
-        <v>C8</v>
-      </c>
-      <c r="E2" t="str">
-        <f>DEC2HEX(202085+B1)</f>
-        <v>31565</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B43" si="0">HEX2DEC(A3)</f>
-        <v>428</v>
-      </c>
-      <c r="C3">
-        <f>B3-B2</f>
-        <v>228</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D43" si="1">DEC2HEX(C3)</f>
-        <v>E4</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E43" si="2">DEC2HEX(202085+B2)</f>
-        <v>3162D</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>294</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>660</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C43" si="3">B4-B3</f>
-        <v>232</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="1"/>
-        <v>E8</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="2"/>
-        <v>31711</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>382</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>898</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="1"/>
-        <v>EE</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="2"/>
-        <v>317F9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>1132</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="1"/>
-        <v>EA</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="2"/>
-        <v>318E7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>568</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>1384</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="3"/>
-        <v>252</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="1"/>
-        <v>FC</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="2"/>
-        <v>319D1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>652</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>1618</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="1"/>
-        <v>EA</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="2"/>
-        <v>31ACD</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>748</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1864</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="3"/>
-        <v>246</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="1"/>
-        <v>F6</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="2"/>
-        <v>31BB7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>2106</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="3"/>
-        <v>242</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="1"/>
-        <v>F2</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="2"/>
-        <v>31CAD</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>928</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>2344</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="1"/>
-        <v>EE</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="2"/>
-        <v>31D9F</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>2572</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="2"/>
-        <v>31E8D</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>2800</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="2"/>
-        <v>31F71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>154</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>3034</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="1"/>
-        <v>EA</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="2"/>
-        <v>32055</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>3268</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="1"/>
-        <v>EA</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="2"/>
-        <v>3213F</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>3520</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="3"/>
-        <v>252</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="1"/>
-        <v>FC</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="2"/>
-        <v>32229</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3720</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="1"/>
-        <v>C8</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="2"/>
-        <v>32325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>3948</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="2"/>
-        <v>323ED</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>1050</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>4176</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="2"/>
-        <v>324D1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>1134</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>4404</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="2"/>
-        <v>325B5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>1222</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>4642</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="1"/>
-        <v>EE</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="2"/>
-        <v>32699</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>1306</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>4870</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="2"/>
-        <v>32787</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>158</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>5110</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="1"/>
-        <v>F0</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="2"/>
-        <v>3286B</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>5360</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="3"/>
-        <v>250</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="1"/>
-        <v>FA</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="2"/>
-        <v>3295B</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>5598</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="1"/>
-        <v>EE</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="2"/>
-        <v>32A55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>161</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>5826</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="1"/>
-        <v>E4</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="2"/>
-        <v>32B43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>6030</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="3"/>
-        <v>204</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="1"/>
-        <v>CC</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="2"/>
-        <v>32C27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>163</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>6238</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="3"/>
-        <v>208</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="1"/>
-        <v>D0</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="2"/>
-        <v>32CF3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>1946</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>6470</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="3"/>
-        <v>232</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="1"/>
-        <v>E8</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="2"/>
-        <v>32DC3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>6708</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="1"/>
-        <v>EE</v>
-      </c>
-      <c r="E30" t="str">
-        <f t="shared" si="2"/>
-        <v>32EAB</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>6948</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="1"/>
-        <v>F0</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" si="2"/>
-        <v>32F99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>166</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>7198</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="3"/>
-        <v>250</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="1"/>
-        <v>FA</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="2"/>
-        <v>33089</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>7210</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="3"/>
-        <v>12</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="1"/>
-        <v>C</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="2"/>
-        <v>33183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>7446</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="1"/>
-        <v>EC</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="2"/>
-        <v>3318F</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>7682</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="1"/>
-        <v>EC</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="2"/>
-        <v>3327B</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>169</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>7912</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="3"/>
-        <v>230</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="1"/>
-        <v>E6</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="2"/>
-        <v>33367</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>170</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>8148</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="1"/>
-        <v>EC</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="2"/>
-        <v>3344D</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>171</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>8392</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="3"/>
-        <v>244</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="1"/>
-        <v>F4</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="2"/>
-        <v>33539</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>8628</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="1"/>
-        <v>EC</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="2"/>
-        <v>3362D</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>8763</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="3"/>
-        <v>135</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="2"/>
-        <v>33719</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>174</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>8898</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="3"/>
-        <v>135</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="2"/>
-        <v>337A0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>175</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>9134</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="1"/>
-        <v>EC</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="2"/>
-        <v>33827</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>2498</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>9368</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="1"/>
-        <v>EA</v>
-      </c>
-      <c r="E43" t="str">
-        <f t="shared" si="2"/>
-        <v>33913</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -29306,7 +28419,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:G68" si="0">IFERROR(HEX2DEC(MID($A$1,A5+1,2)),B4)</f>
+        <f t="shared" ref="B5:B68" si="0">IFERROR(HEX2DEC(MID($A$1,A5+1,2)),B4)</f>
         <v>40</v>
       </c>
       <c r="C5">
@@ -32226,7 +31339,7 @@
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A151">
-        <f t="shared" ref="A151:A214" si="6">A150+4</f>
+        <f t="shared" ref="A151:A153" si="6">A150+4</f>
         <v>589</v>
       </c>
       <c r="B151">
@@ -32258,4 +31371,2500 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2">
+        <f>HEX2DEC(A2)</f>
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>200</v>
+      </c>
+      <c r="D2" t="str">
+        <f>DEC2HEX(C2)</f>
+        <v>C8</v>
+      </c>
+      <c r="E2" t="str">
+        <f>DEC2HEX(202085+B1)</f>
+        <v>31565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B43" si="0">HEX2DEC(A3)</f>
+        <v>428</v>
+      </c>
+      <c r="C3">
+        <f>B3-B2</f>
+        <v>228</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D43" si="1">DEC2HEX(C3)</f>
+        <v>E4</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E43" si="2">DEC2HEX(202085+B2)</f>
+        <v>3162D</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>294</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C43" si="3">B4-B3</f>
+        <v>232</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>E8</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>31711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>382</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>898</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>317F9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>1132</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>318E7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>568</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1384</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>252</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>FC</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>319D1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>652</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1618</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>31ACD</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>748</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1864</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>246</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>F6</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>31BB7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>2106</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>242</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>F2</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>31CAD</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>928</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>2344</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>31D9F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>2572</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>31E8D</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>31F71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>3034</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>32055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>3268</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>3213F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>3520</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>252</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>FC</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>32229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>3720</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>C8</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>32325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>3948</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>323ED</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>1050</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>4176</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>324D1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>1134</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>4404</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>325B5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>1222</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>4642</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>32699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>1306</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>4870</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>32787</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5110</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>F0</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>3286B</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>5360</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>FA</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>3295B</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>5598</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>32A55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>5826</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>E4</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>32B43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>6030</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>204</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>CC</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>32C27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>6238</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>D0</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>32CF3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>1946</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>6470</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>E8</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>32DC3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>6708</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="3"/>
+        <v>238</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>EE</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>32EAB</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>6948</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>F0</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>32F99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>7198</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>FA</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>33089</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>7210</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>33183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>7446</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>3318F</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>7682</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>3327B</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>7912</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>33367</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>8148</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>3344D</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>8392</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="3"/>
+        <v>244</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>F4</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>33539</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>8628</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>3362D</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>8763</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>33719</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>8898</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>135</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>337A0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>9134</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>236</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>EC</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v>33827</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>2498</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>9368</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>EA</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>33913</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AD17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1">
+        <v>0</v>
+      </c>
+      <c r="V1">
+        <v>0</v>
+      </c>
+      <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Y1">
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <v>0</v>
+      </c>
+      <c r="AA1">
+        <v>0</v>
+      </c>
+      <c r="AB1">
+        <v>0</v>
+      </c>
+      <c r="AC1">
+        <v>0</v>
+      </c>
+      <c r="AD1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>2</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>3</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
+        <v>3</v>
+      </c>
+      <c r="AD6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AD7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>3</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>3</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <v>3</v>
+      </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <v>4</v>
+      </c>
+      <c r="AD8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+      <c r="Z9">
+        <v>4</v>
+      </c>
+      <c r="AA9">
+        <v>4</v>
+      </c>
+      <c r="AB9">
+        <v>4</v>
+      </c>
+      <c r="AC9">
+        <v>4</v>
+      </c>
+      <c r="AD9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>4</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <v>3</v>
+      </c>
+      <c r="Y10">
+        <v>5</v>
+      </c>
+      <c r="Z10">
+        <v>4</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>4</v>
+      </c>
+      <c r="AC10">
+        <v>5</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>4</v>
+      </c>
+      <c r="V11">
+        <v>4</v>
+      </c>
+      <c r="W11">
+        <v>4</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>5</v>
+      </c>
+      <c r="Z11">
+        <v>5</v>
+      </c>
+      <c r="AA11">
+        <v>5</v>
+      </c>
+      <c r="AB11">
+        <v>5</v>
+      </c>
+      <c r="AC11">
+        <v>5</v>
+      </c>
+      <c r="AD11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="R12">
+        <v>3</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <v>4</v>
+      </c>
+      <c r="V12">
+        <v>5</v>
+      </c>
+      <c r="W12">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>4</v>
+      </c>
+      <c r="Y12">
+        <v>6</v>
+      </c>
+      <c r="Z12">
+        <v>5</v>
+      </c>
+      <c r="AA12">
+        <v>6</v>
+      </c>
+      <c r="AB12">
+        <v>5</v>
+      </c>
+      <c r="AC12">
+        <v>6</v>
+      </c>
+      <c r="AD12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
+      <c r="X13">
+        <v>5</v>
+      </c>
+      <c r="Y13">
+        <v>6</v>
+      </c>
+      <c r="Z13">
+        <v>6</v>
+      </c>
+      <c r="AA13">
+        <v>6</v>
+      </c>
+      <c r="AB13">
+        <v>6</v>
+      </c>
+      <c r="AC13">
+        <v>6</v>
+      </c>
+      <c r="AD13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <v>6</v>
+      </c>
+      <c r="T14">
+        <v>5</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+      <c r="W14">
+        <v>6</v>
+      </c>
+      <c r="X14">
+        <v>5</v>
+      </c>
+      <c r="Y14">
+        <v>7</v>
+      </c>
+      <c r="Z14">
+        <v>6</v>
+      </c>
+      <c r="AA14">
+        <v>7</v>
+      </c>
+      <c r="AB14">
+        <v>6</v>
+      </c>
+      <c r="AC14">
+        <v>7</v>
+      </c>
+      <c r="AD14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <v>6</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>6</v>
+      </c>
+      <c r="V15">
+        <v>6</v>
+      </c>
+      <c r="W15">
+        <v>6</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>7</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AA15">
+        <v>7</v>
+      </c>
+      <c r="AB15">
+        <v>7</v>
+      </c>
+      <c r="AC15">
+        <v>7</v>
+      </c>
+      <c r="AD15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <v>7</v>
+      </c>
+      <c r="T16">
+        <v>6</v>
+      </c>
+      <c r="U16">
+        <v>6</v>
+      </c>
+      <c r="V16">
+        <v>7</v>
+      </c>
+      <c r="W16">
+        <v>6</v>
+      </c>
+      <c r="X16">
+        <v>6</v>
+      </c>
+      <c r="Y16">
+        <v>8</v>
+      </c>
+      <c r="Z16">
+        <v>7</v>
+      </c>
+      <c r="AA16">
+        <v>8</v>
+      </c>
+      <c r="AB16">
+        <v>7</v>
+      </c>
+      <c r="AC16">
+        <v>8</v>
+      </c>
+      <c r="AD16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17">
+        <v>5</v>
+      </c>
+      <c r="S17">
+        <v>7</v>
+      </c>
+      <c r="T17">
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+      <c r="V17">
+        <v>7</v>
+      </c>
+      <c r="W17">
+        <v>7</v>
+      </c>
+      <c r="X17">
+        <v>6</v>
+      </c>
+      <c r="Y17">
+        <v>8</v>
+      </c>
+      <c r="Z17">
+        <v>8</v>
+      </c>
+      <c r="AA17">
+        <v>8</v>
+      </c>
+      <c r="AB17">
+        <v>8</v>
+      </c>
+      <c r="AC17">
+        <v>8</v>
+      </c>
+      <c r="AD17">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AD17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>